<commit_message>
Updates for version 3 compatibility
Signed-off-by: Gary O'Neall <gary@sourceauditor.com>
</commit_message>
<xml_diff>
--- a/TestFiles/SPDXSpreadsheetExample-2.0.xlsx
+++ b/TestFiles/SPDXSpreadsheetExample-2.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gary\git\Spdx-Java-Spreadsheet-Store\spdx-spreadsheet-store\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gary\git\spdx-java-spreadsheet-store\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAD2826-C3A4-4665-8C87-B77BD495F7CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D8481D-1750-4407-9C9B-66A5E89E6194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Info" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="168">
   <si>
     <t>Spreadsheet Version</t>
   </si>
@@ -630,6 +630,15 @@
   </si>
   <si>
     <t>./package.spdx</t>
+  </si>
+  <si>
+    <t>2010-02-10T00:00:00Z</t>
+  </si>
+  <si>
+    <t>REVIEW</t>
+  </si>
+  <si>
+    <t>2011-03-13T00:00:00Z</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1060,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="20" style="2" customWidth="1"/>
     <col min="2" max="2" width="16" style="2" customWidth="1"/>
@@ -1068,7 +1077,7 @@
     <col min="14" max="14" width="60" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1112,7 +1121,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -1153,7 +1162,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="H3" s="3" t="s">
         <v>76</v>
       </c>
@@ -1161,7 +1170,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="K4" s="3" t="s">
         <v>67</v>
       </c>
@@ -1177,11 +1186,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="30" style="3" customWidth="1"/>
     <col min="2" max="3" width="17" style="3" customWidth="1"/>
@@ -1198,7 +1207,7 @@
     <col min="20" max="20" width="50" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
@@ -1260,7 +1269,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="38.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>78</v>
       </c>
@@ -1332,7 +1341,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="15" style="2" customWidth="1"/>
     <col min="2" max="2" width="120" customWidth="1"/>
@@ -1341,7 +1350,7 @@
     <col min="6" max="6" width="50" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>34</v>
       </c>
@@ -1361,7 +1370,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>95</v>
       </c>
@@ -1378,7 +1387,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>100</v>
       </c>
@@ -1386,7 +1395,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>102</v>
       </c>
@@ -1394,7 +1403,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>104</v>
       </c>
@@ -1402,7 +1411,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>106</v>
       </c>
@@ -1423,7 +1432,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="60" style="3" customWidth="1"/>
     <col min="2" max="3" width="25" style="2" customWidth="1"/>
@@ -1436,7 +1445,7 @@
     <col min="12" max="17" width="60" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>39</v>
       </c>
@@ -1489,7 +1498,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>113</v>
       </c>
@@ -1533,7 +1542,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>123</v>
       </c>
@@ -1580,7 +1589,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="127.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>132</v>
       </c>
@@ -1624,7 +1633,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>141</v>
       </c>
@@ -1669,7 +1678,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="20" style="2" customWidth="1"/>
     <col min="2" max="2" width="25" style="2" customWidth="1"/>
@@ -1678,7 +1687,7 @@
     <col min="5" max="5" width="50" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>52</v>
       </c>
@@ -1695,7 +1704,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>72</v>
       </c>
@@ -1706,7 +1715,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>72</v>
       </c>
@@ -1717,7 +1726,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>72</v>
       </c>
@@ -1728,7 +1737,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>72</v>
       </c>
@@ -1739,7 +1748,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>120</v>
       </c>
@@ -1750,7 +1759,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>76</v>
       </c>
@@ -1770,11 +1779,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="25" style="2" customWidth="1"/>
     <col min="2" max="2" width="70" style="3" customWidth="1"/>
@@ -1784,7 +1795,7 @@
     <col min="6" max="6" width="50" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>56</v>
       </c>
@@ -1804,7 +1815,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>72</v>
       </c>
@@ -1821,37 +1832,71 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>154</v>
       </c>
     </row>
@@ -1868,14 +1913,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="60" style="3" customWidth="1"/>
     <col min="2" max="2" width="20" style="2" customWidth="1"/>
     <col min="3" max="3" width="120" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>61</v>
       </c>
@@ -1886,7 +1931,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>160</v>
       </c>
@@ -1897,7 +1942,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>162</v>
       </c>

</xml_diff>